<commit_message>
1nf changed date format
</commit_message>
<xml_diff>
--- a/Assessment/1NF.xlsx
+++ b/Assessment/1NF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sufi/Desktop/DB/Assessment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72F007D-628E-E242-9A1F-296B8211E029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DCA404-42EE-2D47-88CE-67D1C5995CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -744,6 +744,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -868,16 +871,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -890,6 +887,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -914,8 +917,9 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1211,7 +1215,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -1402,16 +1405,16 @@
   <tableColumns count="12">
     <tableColumn id="2" xr3:uid="{102CD81C-6101-834C-AB81-49A846155353}" name="name" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{CAAE91BC-0350-B749-99CA-4308FA528B2D}" name="email" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{3A1A00D8-707A-A04B-8DD2-56F01CAF86B3}" name="dob" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{B9A6793D-8220-EE47-950C-90306299014C}" name="street" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{631C84EA-5293-3D43-B623-6AE4D94117AC}" name="city" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{FF2E1812-C9D4-224C-8C4F-389F20CBEBA0}" name="country" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{665C12C4-7BF2-854B-AFD1-9ECF79D23824}" name="zipcode" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{DA316161-0013-4D41-88DC-92AB1DBDC0E1}" name="favorite_book" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{F4A6C82F-ABEA-C342-9B01-B755B7B52C52}" name="favorite_drink" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{95FBF865-CDA5-A841-BA06-60B12F13187B}" name="favorite_activity" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{A1A8A415-1E82-364C-9779-3AD3F13B25E2}" name="neighbour" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{34077D9F-1FFD-E849-AEFD-91239A928499}" name="neighbour_email" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{3A1A00D8-707A-A04B-8DD2-56F01CAF86B3}" name="dob" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{B9A6793D-8220-EE47-950C-90306299014C}" name="street" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{631C84EA-5293-3D43-B623-6AE4D94117AC}" name="city" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{FF2E1812-C9D4-224C-8C4F-389F20CBEBA0}" name="country" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{665C12C4-7BF2-854B-AFD1-9ECF79D23824}" name="zipcode" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{DA316161-0013-4D41-88DC-92AB1DBDC0E1}" name="favorite_book" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{F4A6C82F-ABEA-C342-9B01-B755B7B52C52}" name="favorite_drink" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{95FBF865-CDA5-A841-BA06-60B12F13187B}" name="favorite_activity" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{A1A8A415-1E82-364C-9779-3AD3F13B25E2}" name="neighbour" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{34077D9F-1FFD-E849-AEFD-91239A928499}" name="neighbour_email" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1709,14 +1712,14 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="2" bestFit="1" customWidth="1"/>
@@ -1730,40 +1733,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="7" t="s">
         <v>238</v>
       </c>
     </row>
@@ -1774,7 +1777,7 @@
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="10">
         <v>34773</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1812,7 +1815,7 @@
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="10">
         <v>34774</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1839,7 +1842,7 @@
       <c r="K3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1850,7 +1853,7 @@
       <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="10">
         <v>34142</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1888,7 +1891,7 @@
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="10">
         <v>34142</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1915,7 +1918,7 @@
       <c r="K5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1926,7 +1929,7 @@
       <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="10">
         <v>33491</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1964,7 +1967,7 @@
       <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="10">
         <v>33492</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -1991,7 +1994,7 @@
       <c r="K7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2002,7 +2005,7 @@
       <c r="B8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="10">
         <v>36134</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -2040,7 +2043,7 @@
       <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="10">
         <v>36134</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -2067,7 +2070,7 @@
       <c r="K9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="4" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2078,7 +2081,7 @@
       <c r="B10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="10">
         <v>30650</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -2116,7 +2119,7 @@
       <c r="B11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="10">
         <v>30651</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -2143,7 +2146,7 @@
       <c r="K11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="L11" s="4" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2154,7 +2157,7 @@
       <c r="B12" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="10">
         <v>32707</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -2192,7 +2195,7 @@
       <c r="B13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="10">
         <v>32707</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -2219,7 +2222,7 @@
       <c r="K13" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L13" s="4" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2230,7 +2233,7 @@
       <c r="B14" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="10">
         <v>35180</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -2268,7 +2271,7 @@
       <c r="B15" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="10">
         <v>35180</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -2295,7 +2298,7 @@
       <c r="K15" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="L15" s="4" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2306,7 +2309,7 @@
       <c r="B16" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="10">
         <v>32882</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -2344,7 +2347,7 @@
       <c r="B17" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="10">
         <v>32882</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -2371,7 +2374,7 @@
       <c r="K17" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="L17" s="4" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2382,7 +2385,7 @@
       <c r="B18" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="10">
         <v>34198</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -2420,7 +2423,7 @@
       <c r="B19" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="10">
         <v>34198</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -2447,7 +2450,7 @@
       <c r="K19" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="L19" s="4" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2458,7 +2461,7 @@
       <c r="B20" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="10">
         <v>35725</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -2496,7 +2499,7 @@
       <c r="B21" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="10">
         <v>35726</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -2523,7 +2526,7 @@
       <c r="K21" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="L21" s="4" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2534,7 +2537,7 @@
       <c r="B22" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="10">
         <v>33737</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -2572,7 +2575,7 @@
       <c r="B23" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="10">
         <v>33738</v>
       </c>
       <c r="D23" s="3" t="s">
@@ -2599,7 +2602,7 @@
       <c r="K23" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="L23" s="5" t="s">
+      <c r="L23" s="4" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2610,7 +2613,7 @@
       <c r="B24" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="10">
         <v>31470</v>
       </c>
       <c r="D24" s="3" t="s">
@@ -2648,7 +2651,7 @@
       <c r="B25" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="10">
         <v>31470</v>
       </c>
       <c r="D25" s="3" t="s">
@@ -2675,7 +2678,7 @@
       <c r="K25" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="L25" s="4" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2686,7 +2689,7 @@
       <c r="B26" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="10">
         <v>33567</v>
       </c>
       <c r="D26" s="3" t="s">
@@ -2724,7 +2727,7 @@
       <c r="B27" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="10">
         <v>33567</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -2751,7 +2754,7 @@
       <c r="K27" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="L27" s="4" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2762,7 +2765,7 @@
       <c r="B28" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="10">
         <v>31809</v>
       </c>
       <c r="D28" s="3" t="s">
@@ -2800,7 +2803,7 @@
       <c r="B29" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="10">
         <v>31809</v>
       </c>
       <c r="D29" s="3" t="s">
@@ -2827,7 +2830,7 @@
       <c r="K29" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="L29" s="4" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2838,7 +2841,7 @@
       <c r="B30" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="10">
         <v>30906</v>
       </c>
       <c r="D30" s="3" t="s">
@@ -2876,7 +2879,7 @@
       <c r="B31" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="10">
         <v>30906</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -2903,7 +2906,7 @@
       <c r="K31" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="L31" s="5" t="s">
+      <c r="L31" s="4" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2914,7 +2917,7 @@
       <c r="B32" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="10">
         <v>32941</v>
       </c>
       <c r="D32" s="3" t="s">
@@ -2952,7 +2955,7 @@
       <c r="B33" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="10">
         <v>32941</v>
       </c>
       <c r="D33" s="3" t="s">
@@ -2979,7 +2982,7 @@
       <c r="K33" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="L33" s="4" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2990,7 +2993,7 @@
       <c r="B34" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="10">
         <v>35020</v>
       </c>
       <c r="D34" s="3" t="s">
@@ -3028,7 +3031,7 @@
       <c r="B35" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="10">
         <v>35020</v>
       </c>
       <c r="D35" s="3" t="s">
@@ -3055,7 +3058,7 @@
       <c r="K35" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="L35" s="5" t="s">
+      <c r="L35" s="4" t="s">
         <v>193</v>
       </c>
     </row>
@@ -3066,7 +3069,7 @@
       <c r="B36" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="10">
         <v>34505</v>
       </c>
       <c r="D36" s="3" t="s">
@@ -3104,7 +3107,7 @@
       <c r="B37" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="10">
         <v>34505</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -3131,7 +3134,7 @@
       <c r="K37" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="L37" s="5" t="s">
+      <c r="L37" s="4" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3142,7 +3145,7 @@
       <c r="B38" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="10">
         <v>33949</v>
       </c>
       <c r="D38" s="3" t="s">
@@ -3180,7 +3183,7 @@
       <c r="B39" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="10">
         <v>33949</v>
       </c>
       <c r="D39" s="3" t="s">
@@ -3207,83 +3210,83 @@
       <c r="K39" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="L39" s="5" t="s">
+      <c r="L39" s="4" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:12" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="11">
         <v>32411</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="E40" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="F40" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="G40" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="H40" s="6" t="s">
+      <c r="H40" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="I40" s="6" t="s">
+      <c r="I40" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="J40" s="6" t="s">
+      <c r="J40" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K40" s="6" t="s">
+      <c r="K40" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="L40" s="8" t="s">
+      <c r="L40" s="6" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="41" spans="1:12" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="11">
         <v>32411</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="E41" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="F41" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="G41" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="H41" s="6" t="s">
+      <c r="H41" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="I41" s="6" t="s">
+      <c r="I41" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="J41" s="6" t="s">
+      <c r="J41" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K41" s="6" t="s">
+      <c r="K41" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="L41" s="6" t="s">
+      <c r="L41" s="5" t="s">
         <v>219</v>
       </c>
     </row>

</xml_diff>